<commit_message>
added additional analyses (sig test for semipartials)
</commit_message>
<xml_diff>
--- a/output/facet-wellbeing-tables.xlsx
+++ b/output/facet-wellbeing-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="480" windowWidth="24860" windowHeight="15580" tabRatio="644" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="5520" yWindow="5200" windowWidth="24860" windowHeight="15580" tabRatio="644" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="descriptives" sheetId="7" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="incrementalrsquare" sheetId="10" r:id="rId7"/>
     <sheet name="zero-order" sheetId="11" r:id="rId8"/>
     <sheet name="semipartials" sheetId="3" r:id="rId9"/>
+    <sheet name="semipartial_p" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="129">
   <si>
     <t>swl</t>
   </si>
@@ -480,9 +481,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode=".00"/>
-    <numFmt numFmtId="166" formatCode="0."/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode=".00"/>
+    <numFmt numFmtId="165" formatCode="0."/>
+    <numFmt numFmtId="166" formatCode=".000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -628,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,8 +823,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,52 +849,55 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -979,6 +993,10 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1074,6 +1092,10 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2069,6 +2091,311 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:J31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV51"/>
@@ -2083,52 +2410,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
-      <c r="AK1" s="43"/>
-      <c r="AL1" s="43"/>
-      <c r="AM1" s="43"/>
-      <c r="AN1" s="43"/>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AQ1" s="43"/>
-      <c r="AR1" s="43"/>
-      <c r="AS1" s="43"/>
-      <c r="AT1" s="43"/>
-      <c r="AU1" s="43"/>
-      <c r="AV1" s="43"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" s="1" customFormat="1" ht="90">
       <c r="B2" s="1" t="s">
@@ -8698,22 +9025,22 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="78" customHeight="1">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
     </row>
     <row r="51" spans="1:6" ht="100" customHeight="1">
-      <c r="A51" s="42"/>
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
+      <c r="A51" s="45"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9234,7 +9561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -9820,13 +10147,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="28"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="28" t="s">
         <v>127</v>
       </c>
@@ -10112,13 +10439,13 @@
       <c r="A1" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="28" t="s">
         <v>105</v>
       </c>
@@ -10365,15 +10692,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="21" t="s">
         <v>106</v>
       </c>
@@ -10396,228 +10723,229 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="22">
-        <v>0.4</v>
-      </c>
-      <c r="C2" s="22">
-        <v>0.51600000000000001</v>
+      <c r="B2" s="42">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="C2" s="42">
+        <v>0.51800000000000002</v>
       </c>
       <c r="D2" s="22">
         <v>0.11700000000000001</v>
       </c>
       <c r="E2" s="22">
-        <v>5.8999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F2" s="22">
-        <v>0.187</v>
+        <v>0.182</v>
       </c>
       <c r="G2" s="21" t="str">
         <f>D2&amp;" ("&amp;E2&amp;" to "&amp;F2&amp;")"</f>
-        <v>0.117 (0.059 to 0.187)</v>
+        <v>0.117 (0.056 to 0.182)</v>
       </c>
       <c r="J2" s="41">
         <f>AVERAGE(B2:B4)</f>
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>0.48100000000000004</v>
+      </c>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="22">
-        <v>0.47</v>
-      </c>
-      <c r="C3" s="22">
-        <v>0.503</v>
+      <c r="B3" s="42">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="C3" s="42">
+        <v>0.505</v>
       </c>
       <c r="D3" s="22">
         <v>3.9E-2</v>
       </c>
       <c r="E3" s="22">
-        <v>0.02</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="F3" s="22">
-        <v>9.2999999999999999E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="G3" s="21" t="str">
         <f t="shared" ref="G3:G10" si="0">D3&amp;" ("&amp;E3&amp;" to "&amp;F3&amp;")"</f>
-        <v>0.039 (0.02 to 0.093)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>0.039 (-0.008 to 0.089)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="22">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C4" s="22">
-        <v>0.58799999999999997</v>
+      <c r="B4" s="42">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="C4" s="42">
+        <v>0.58899999999999997</v>
       </c>
       <c r="D4" s="22">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="E4" s="22">
-        <v>-1.6E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="F4" s="22">
-        <v>6.2E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G4" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.013 (-0.016 to 0.062)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>0.013 (-0.022 to 0.049)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="22">
-        <v>0.495</v>
-      </c>
-      <c r="C5" s="22">
-        <v>0.56499999999999995</v>
+      <c r="B5" s="42">
+        <v>0.497</v>
+      </c>
+      <c r="C5" s="42">
+        <v>0.56699999999999995</v>
       </c>
       <c r="D5" s="22">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E5" s="22">
-        <v>4.7E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F5" s="22">
-        <v>0.129</v>
+        <v>0.127</v>
       </c>
       <c r="G5" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.07 (0.047 to 0.129)</v>
-      </c>
-      <c r="J5" s="12">
+        <v>0.07 (0.024 to 0.127)</v>
+      </c>
+      <c r="J5" s="43">
         <f>AVERAGE(B5:B10)</f>
-        <v>0.54916666666666669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>0.55066666666666675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="22">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="C6" s="22">
-        <v>0.497</v>
+      <c r="B6" s="42">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="C6" s="42">
+        <v>0.499</v>
       </c>
       <c r="D6" s="22">
         <v>0.13500000000000001</v>
       </c>
       <c r="E6" s="22">
-        <v>0.106</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="F6" s="22">
-        <v>0.20499999999999999</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="G6" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.135 (0.106 to 0.205)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>0.135 (0.069 to 0.209)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="22">
-        <v>0.68100000000000005</v>
-      </c>
-      <c r="C7" s="22">
-        <v>0.72599999999999998</v>
+      <c r="B7" s="42">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="C7" s="42">
+        <v>0.72699999999999998</v>
       </c>
       <c r="D7" s="22">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E7" s="22">
-        <v>2.1000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F7" s="22">
-        <v>6.6000000000000003E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="G7" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.044 (0.021 to 0.066)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.044 (0.011 to 0.079)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="22">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="C8" s="22">
-        <v>0.58399999999999996</v>
+      <c r="B8" s="42">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0.58599999999999997</v>
       </c>
       <c r="D8" s="22">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="E8" s="22">
-        <v>4.7E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F8" s="22">
-        <v>0.10199999999999999</v>
+        <v>0.128</v>
       </c>
       <c r="G8" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.071 (0.047 to 0.102)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>0.071 (0.022 to 0.128)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="22">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="C9" s="22">
-        <v>0.72299999999999998</v>
+      <c r="B9" s="42">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="C9" s="42">
+        <v>0.72399999999999998</v>
       </c>
       <c r="D9" s="22">
         <v>0.106</v>
       </c>
       <c r="E9" s="22">
-        <v>9.0999999999999998E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F9" s="22">
-        <v>0.14299999999999999</v>
+        <v>0.151</v>
       </c>
       <c r="G9" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.106 (0.091 to 0.143)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>0.106 (0.065 to 0.151)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="22">
-        <v>0.627</v>
-      </c>
-      <c r="C10" s="22">
-        <v>0.77600000000000002</v>
+      <c r="B10" s="42">
+        <v>0.628</v>
+      </c>
+      <c r="C10" s="42">
+        <v>0.77700000000000002</v>
       </c>
       <c r="D10" s="22">
         <v>0.14899999999999999</v>
       </c>
       <c r="E10" s="22">
-        <v>0.114</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F10" s="22">
-        <v>0.19600000000000001</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="G10" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0.149 (0.114 to 0.196)</v>
+        <v>0.149 (0.102 to 0.199)</v>
       </c>
     </row>
   </sheetData>
@@ -13994,24 +14322,24 @@
       <c r="C32" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="143" customHeight="1">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
     </row>
     <row r="36" spans="1:6" ht="109" customHeight="1">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>